<commit_message>
updated sprint tracking spreadsheet for US01
</commit_message>
<xml_diff>
--- a/Team07Report.xlsx
+++ b/Team07Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18048\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liamb\OneDrive\Desktop\SSW-555\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47827DF4-A3A5-4FD5-AF41-06640D55DF6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF14B6D-2FDD-457F-9773-4D85A4F78A0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -2029,15 +2028,15 @@
       <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.8203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.46875" customWidth="1"/>
-    <col min="3" max="3" width="8.46875" customWidth="1"/>
-    <col min="4" max="5" width="20.46875" customWidth="1"/>
+    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2054,7 +2053,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>176</v>
       </c>
@@ -2071,7 +2070,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>181</v>
       </c>
@@ -2088,7 +2087,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>186</v>
       </c>
@@ -2105,7 +2104,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>190</v>
       </c>
@@ -2122,7 +2121,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>196</v>
       </c>
@@ -2139,7 +2138,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>201</v>
       </c>
@@ -2156,7 +2155,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>205</v>
       </c>
@@ -2173,7 +2172,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
@@ -2209,16 +2208,16 @@
       <selection activeCell="D2" sqref="D2:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.17578125" customWidth="1"/>
-    <col min="2" max="2" width="7.64453125" customWidth="1"/>
-    <col min="3" max="3" width="35.52734375" customWidth="1"/>
-    <col min="4" max="4" width="6.64453125" customWidth="1"/>
-    <col min="5" max="5" width="7.64453125" customWidth="1"/>
+    <col min="1" max="1" width="5.125" customWidth="1"/>
+    <col min="2" max="2" width="7.625" customWidth="1"/>
+    <col min="3" max="3" width="35.5" customWidth="1"/>
+    <col min="4" max="4" width="6.625" customWidth="1"/>
+    <col min="5" max="5" width="7.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2235,7 +2234,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2252,7 +2251,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2269,7 +2268,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2286,7 +2285,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2303,7 +2302,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2320,7 +2319,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2337,7 +2336,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2354,7 +2353,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2371,7 +2370,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2388,7 +2387,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2405,7 +2404,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2422,7 +2421,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2439,7 +2438,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -2456,7 +2455,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -2473,7 +2472,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2490,7 +2489,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2507,7 +2506,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2524,7 +2523,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2541,7 +2540,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2558,7 +2557,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -2575,7 +2574,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2</v>
       </c>
@@ -2592,7 +2591,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
@@ -2609,7 +2608,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2</v>
       </c>
@@ -2626,7 +2625,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2</v>
       </c>
@@ -2643,7 +2642,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2</v>
       </c>
@@ -2660,7 +2659,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2</v>
       </c>
@@ -2677,7 +2676,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2</v>
       </c>
@@ -2694,7 +2693,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2</v>
       </c>
@@ -2711,7 +2710,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3</v>
       </c>
@@ -2728,7 +2727,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3</v>
       </c>
@@ -2745,7 +2744,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3</v>
       </c>
@@ -2762,7 +2761,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3</v>
       </c>
@@ -2779,7 +2778,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2796,7 +2795,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3</v>
       </c>
@@ -2813,7 +2812,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2830,7 +2829,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>3</v>
       </c>
@@ -2847,7 +2846,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2864,7 +2863,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2881,7 +2880,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2898,7 +2897,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>3</v>
       </c>
@@ -2915,7 +2914,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2932,7 +2931,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2964,47 +2963,47 @@
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.8203125" style="7"/>
-    <col min="2" max="2" width="9.46875" customWidth="1"/>
-    <col min="3" max="3" width="15.8203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3515625" customWidth="1"/>
-    <col min="5" max="5" width="6.8203125" customWidth="1"/>
-    <col min="6" max="6" width="12.46875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="7"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>161</v>
       </c>
@@ -3027,7 +3026,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>162</v>
       </c>
@@ -3043,7 +3042,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>163</v>
       </c>
@@ -3068,7 +3067,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>164</v>
       </c>
@@ -3093,7 +3092,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>165</v>
       </c>
@@ -3118,7 +3117,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>166</v>
       </c>
@@ -3158,17 +3157,17 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.8203125" style="2"/>
-    <col min="2" max="2" width="16.64453125" customWidth="1"/>
-    <col min="3" max="3" width="12.46875" customWidth="1"/>
-    <col min="4" max="4" width="7.17578125" customWidth="1"/>
-    <col min="5" max="5" width="6.8203125" customWidth="1"/>
-    <col min="6" max="6" width="12.46875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="2"/>
+    <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3188,7 +3187,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>42633</v>
       </c>
@@ -3199,7 +3198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F3" s="9">
         <f>D5</f>
         <v>0</v>
@@ -3218,21 +3217,21 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.64453125" customWidth="1"/>
-    <col min="2" max="2" width="24.46875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.64453125" customWidth="1"/>
-    <col min="5" max="5" width="8.64453125" customWidth="1"/>
-    <col min="6" max="7" width="8.8203125" customWidth="1"/>
-    <col min="8" max="8" width="10.87890625" customWidth="1"/>
-    <col min="9" max="9" width="10.8203125" style="6"/>
+    <col min="1" max="1" width="7.625" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.625" customWidth="1"/>
+    <col min="5" max="5" width="8.625" customWidth="1"/>
+    <col min="6" max="7" width="8.875" customWidth="1"/>
+    <col min="8" max="8" width="10.875" customWidth="1"/>
+    <col min="9" max="9" width="10.875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3261,7 +3260,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -3280,8 +3279,17 @@
       <c r="F2">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>40</v>
+      </c>
+      <c r="H2">
+        <v>30</v>
+      </c>
+      <c r="I2" s="6">
+        <v>42640</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -3300,8 +3308,9 @@
       <c r="F3">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -3321,7 +3330,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -3341,7 +3350,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -3361,7 +3370,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -3381,7 +3390,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -3401,7 +3410,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -3421,7 +3430,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -3441,7 +3450,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -3461,7 +3470,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -3481,7 +3490,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -3501,7 +3510,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -3522,7 +3531,7 @@
       </c>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -3542,21 +3551,21 @@
         <v>180</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>30</v>
       </c>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="5"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
         <v>32</v>
       </c>
@@ -3576,9 +3585,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3622,9 +3631,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3667,9 +3676,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3708,17 +3717,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.17578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.46875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>113</v>
       </c>
@@ -3729,7 +3738,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -3740,7 +3749,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -3751,7 +3760,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -3762,7 +3771,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -3773,7 +3782,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -3784,7 +3793,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -3795,7 +3804,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -3806,7 +3815,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -3817,7 +3826,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -3828,7 +3837,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -3839,7 +3848,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -3850,7 +3859,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -3861,7 +3870,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -3872,7 +3881,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -3883,7 +3892,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -3894,7 +3903,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -3905,7 +3914,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -3916,7 +3925,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -3927,7 +3936,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -3938,7 +3947,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -3949,7 +3958,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>134</v>
       </c>
@@ -3960,7 +3969,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>135</v>
       </c>
@@ -3971,7 +3980,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -3982,7 +3991,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -3993,7 +4002,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>138</v>
       </c>
@@ -4004,7 +4013,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="126" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -4015,7 +4024,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -4026,7 +4035,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -4037,7 +4046,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -4048,7 +4057,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>143</v>
       </c>
@@ -4059,7 +4068,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -4070,7 +4079,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -4081,7 +4090,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -4092,7 +4101,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -4103,7 +4112,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -4114,7 +4123,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -4125,7 +4134,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -4136,7 +4145,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -4147,7 +4156,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -4158,7 +4167,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -4169,7 +4178,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -4180,7 +4189,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
updated sprint tracking spreadsheet for US10
</commit_message>
<xml_diff>
--- a/Team07Report.xlsx
+++ b/Team07Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18048\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liamb\OneDrive\Desktop\SSW-555\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47827DF4-A3A5-4FD5-AF41-06640D55DF6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07689875-6082-400F-A5D0-F98FF5806B31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -2029,15 +2028,15 @@
       <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.8203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.46875" customWidth="1"/>
-    <col min="3" max="3" width="8.46875" customWidth="1"/>
-    <col min="4" max="5" width="20.46875" customWidth="1"/>
+    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2054,7 +2053,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>176</v>
       </c>
@@ -2071,7 +2070,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>181</v>
       </c>
@@ -2088,7 +2087,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>186</v>
       </c>
@@ -2105,7 +2104,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>190</v>
       </c>
@@ -2122,7 +2121,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>196</v>
       </c>
@@ -2139,7 +2138,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>201</v>
       </c>
@@ -2156,7 +2155,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>205</v>
       </c>
@@ -2173,7 +2172,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
@@ -2209,16 +2208,16 @@
       <selection activeCell="D2" sqref="D2:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.17578125" customWidth="1"/>
-    <col min="2" max="2" width="7.64453125" customWidth="1"/>
-    <col min="3" max="3" width="35.52734375" customWidth="1"/>
-    <col min="4" max="4" width="6.64453125" customWidth="1"/>
-    <col min="5" max="5" width="7.64453125" customWidth="1"/>
+    <col min="1" max="1" width="5.125" customWidth="1"/>
+    <col min="2" max="2" width="7.625" customWidth="1"/>
+    <col min="3" max="3" width="35.5" customWidth="1"/>
+    <col min="4" max="4" width="6.625" customWidth="1"/>
+    <col min="5" max="5" width="7.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2235,7 +2234,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2252,7 +2251,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2269,7 +2268,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2286,7 +2285,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2303,7 +2302,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2320,7 +2319,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2337,7 +2336,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2354,7 +2353,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2371,7 +2370,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2388,7 +2387,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2405,7 +2404,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2422,7 +2421,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2439,7 +2438,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -2456,7 +2455,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -2473,7 +2472,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2490,7 +2489,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2507,7 +2506,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2524,7 +2523,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2541,7 +2540,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2558,7 +2557,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -2575,7 +2574,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2</v>
       </c>
@@ -2592,7 +2591,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
@@ -2609,7 +2608,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2</v>
       </c>
@@ -2626,7 +2625,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2</v>
       </c>
@@ -2643,7 +2642,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2</v>
       </c>
@@ -2660,7 +2659,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2</v>
       </c>
@@ -2677,7 +2676,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2</v>
       </c>
@@ -2694,7 +2693,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2</v>
       </c>
@@ -2711,7 +2710,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3</v>
       </c>
@@ -2728,7 +2727,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3</v>
       </c>
@@ -2745,7 +2744,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3</v>
       </c>
@@ -2762,7 +2761,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3</v>
       </c>
@@ -2779,7 +2778,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2796,7 +2795,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3</v>
       </c>
@@ -2813,7 +2812,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2830,7 +2829,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>3</v>
       </c>
@@ -2847,7 +2846,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2864,7 +2863,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2881,7 +2880,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2898,7 +2897,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>3</v>
       </c>
@@ -2915,7 +2914,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2932,7 +2931,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2964,47 +2963,47 @@
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.8203125" style="7"/>
-    <col min="2" max="2" width="9.46875" customWidth="1"/>
-    <col min="3" max="3" width="15.8203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3515625" customWidth="1"/>
-    <col min="5" max="5" width="6.8203125" customWidth="1"/>
-    <col min="6" max="6" width="12.46875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="7"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>161</v>
       </c>
@@ -3027,7 +3026,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>162</v>
       </c>
@@ -3043,7 +3042,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>163</v>
       </c>
@@ -3068,7 +3067,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>164</v>
       </c>
@@ -3093,7 +3092,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>165</v>
       </c>
@@ -3118,7 +3117,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>166</v>
       </c>
@@ -3158,17 +3157,17 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.8203125" style="2"/>
-    <col min="2" max="2" width="16.64453125" customWidth="1"/>
-    <col min="3" max="3" width="12.46875" customWidth="1"/>
-    <col min="4" max="4" width="7.17578125" customWidth="1"/>
-    <col min="5" max="5" width="6.8203125" customWidth="1"/>
-    <col min="6" max="6" width="12.46875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="2"/>
+    <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3188,7 +3187,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>42633</v>
       </c>
@@ -3199,7 +3198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F3" s="9">
         <f>D5</f>
         <v>0</v>
@@ -3218,21 +3217,21 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.64453125" customWidth="1"/>
-    <col min="2" max="2" width="24.46875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.64453125" customWidth="1"/>
-    <col min="5" max="5" width="8.64453125" customWidth="1"/>
-    <col min="6" max="7" width="8.8203125" customWidth="1"/>
-    <col min="8" max="8" width="10.87890625" customWidth="1"/>
-    <col min="9" max="9" width="10.8203125" style="6"/>
+    <col min="1" max="1" width="7.625" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.625" customWidth="1"/>
+    <col min="5" max="5" width="8.625" customWidth="1"/>
+    <col min="6" max="7" width="8.875" customWidth="1"/>
+    <col min="8" max="8" width="10.875" customWidth="1"/>
+    <col min="9" max="9" width="10.875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3261,7 +3260,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -3281,7 +3280,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -3300,8 +3299,9 @@
       <c r="F3">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -3341,7 +3341,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -3381,7 +3381,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -3441,7 +3441,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -3460,8 +3460,17 @@
       <c r="F11">
         <v>90</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>50</v>
+      </c>
+      <c r="H11">
+        <v>30</v>
+      </c>
+      <c r="I11" s="6">
+        <v>42640</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -3481,7 +3490,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -3501,7 +3510,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -3522,7 +3531,7 @@
       </c>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -3542,21 +3551,21 @@
         <v>180</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>30</v>
       </c>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="5"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
         <v>32</v>
       </c>
@@ -3576,9 +3585,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3622,9 +3631,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3667,9 +3676,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3708,17 +3717,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.17578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.46875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>113</v>
       </c>
@@ -3729,7 +3738,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -3740,7 +3749,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -3751,7 +3760,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -3762,7 +3771,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -3773,7 +3782,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -3784,7 +3793,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -3795,7 +3804,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -3806,7 +3815,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -3817,7 +3826,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -3828,7 +3837,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -3839,7 +3848,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -3850,7 +3859,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -3861,7 +3870,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -3872,7 +3881,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -3883,7 +3892,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -3894,7 +3903,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -3905,7 +3914,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -3916,7 +3925,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -3927,7 +3936,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -3938,7 +3947,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -3949,7 +3958,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>134</v>
       </c>
@@ -3960,7 +3969,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>135</v>
       </c>
@@ -3971,7 +3980,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -3982,7 +3991,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -3993,7 +4002,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>138</v>
       </c>
@@ -4004,7 +4013,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="126" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -4015,7 +4024,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -4026,7 +4035,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -4037,7 +4046,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -4048,7 +4057,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>143</v>
       </c>
@@ -4059,7 +4068,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -4070,7 +4079,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -4081,7 +4090,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -4092,7 +4101,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -4103,7 +4112,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -4114,7 +4123,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -4125,7 +4134,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -4136,7 +4145,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -4147,7 +4156,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -4158,7 +4167,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -4169,7 +4178,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -4180,7 +4189,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>155</v>
       </c>

</xml_diff>